<commit_message>
Correción archivo densidad poblacional
</commit_message>
<xml_diff>
--- a/data/india/population_density_IN.xlsx
+++ b/data/india/population_density_IN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E36C1D8F-6686-4316-A3F7-EA14D8D56A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776BF93C-7A6C-4977-8900-8A2714D30FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E7E294A-2B1B-457B-B9FE-B3636AF373CB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
   <si>
     <t>State Name</t>
   </si>
@@ -48,21 +48,12 @@
     <t>Delhi</t>
   </si>
   <si>
-    <t>16,787,941</t>
-  </si>
-  <si>
     <t>Chandigarh</t>
   </si>
   <si>
-    <t>1,055,450</t>
-  </si>
-  <si>
     <t>Puducherry</t>
   </si>
   <si>
-    <t>1,247,953</t>
-  </si>
-  <si>
     <t>Daman and Diu</t>
   </si>
   <si>
@@ -72,178 +63,94 @@
     <t>Bihar</t>
   </si>
   <si>
-    <t>104,099,452</t>
-  </si>
-  <si>
     <t>West Bengal</t>
   </si>
   <si>
-    <t>91,276,115</t>
-  </si>
-  <si>
     <t>Kerala</t>
   </si>
   <si>
-    <t>33,406,061</t>
-  </si>
-  <si>
     <t>Uttar Pradesh</t>
   </si>
   <si>
-    <t>199,812,341</t>
-  </si>
-  <si>
     <t>Dadra and Nagar Haveli</t>
   </si>
   <si>
     <t>Haryana</t>
   </si>
   <si>
-    <t>25,351,462</t>
-  </si>
-  <si>
     <t>Tamil Nadu</t>
   </si>
   <si>
-    <t>72,147,030</t>
-  </si>
-  <si>
     <t>Punjab</t>
   </si>
   <si>
-    <t>27,743,338</t>
-  </si>
-  <si>
     <t>Jharkhand</t>
   </si>
   <si>
-    <t>32,988,134</t>
-  </si>
-  <si>
     <t>Assam</t>
   </si>
   <si>
-    <t>31,205,576</t>
-  </si>
-  <si>
     <t>Goa</t>
   </si>
   <si>
-    <t>1,458,545</t>
-  </si>
-  <si>
     <t>Maharashtra</t>
   </si>
   <si>
-    <t>112,374,333</t>
-  </si>
-  <si>
     <t>Tripura</t>
   </si>
   <si>
-    <t>3,673,917</t>
-  </si>
-  <si>
     <t>Karnataka</t>
   </si>
   <si>
-    <t>61,095,297</t>
-  </si>
-  <si>
     <t>Andhra Pradesh</t>
   </si>
   <si>
-    <t>84,580,777</t>
-  </si>
-  <si>
     <t>Gujarat</t>
   </si>
   <si>
-    <t>60,439,692</t>
-  </si>
-  <si>
     <t>Telangana</t>
   </si>
   <si>
-    <t>35,193,978</t>
-  </si>
-  <si>
     <t>Orissa</t>
   </si>
   <si>
-    <t>41,974,218</t>
-  </si>
-  <si>
     <t>Madhya Pradesh</t>
   </si>
   <si>
-    <t>72,626,809</t>
-  </si>
-  <si>
     <t>Rajasthan</t>
   </si>
   <si>
-    <t>68,548,437</t>
-  </si>
-  <si>
     <t>Chhattisgarh</t>
   </si>
   <si>
-    <t>25,545,198</t>
-  </si>
-  <si>
     <t>Uttarakhand</t>
   </si>
   <si>
-    <t>10,086,292</t>
-  </si>
-  <si>
     <t>Meghalaya</t>
   </si>
   <si>
-    <t>2,966,889</t>
-  </si>
-  <si>
     <t>Manipur</t>
   </si>
   <si>
-    <t>2,855,794</t>
-  </si>
-  <si>
     <t>Himachal Pradesh</t>
   </si>
   <si>
-    <t>6,864,602</t>
-  </si>
-  <si>
     <t>Nagaland</t>
   </si>
   <si>
-    <t>1,978,502</t>
-  </si>
-  <si>
     <t>Sikkim</t>
   </si>
   <si>
     <t>Jammu and Kashmir</t>
   </si>
   <si>
-    <t>12,541,302</t>
-  </si>
-  <si>
     <t>Mizoram</t>
   </si>
   <si>
-    <t>1,097,206</t>
-  </si>
-  <si>
     <t>Andaman &amp; Nicobar Islands</t>
   </si>
   <si>
     <t>Arunachal Pradesh</t>
-  </si>
-  <si>
-    <t>1,383,727</t>
   </si>
   <si>
     <t>Density Class</t>
@@ -304,10 +211,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,7 +533,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,7 +554,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="E1" s="1"/>
     </row>
@@ -654,543 +562,544 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
+      <c r="B2" s="3">
+        <v>16787941</v>
       </c>
       <c r="C2" s="2">
         <v>11320</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1055450</v>
       </c>
       <c r="C3" s="2">
         <v>9258</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1247953</v>
       </c>
       <c r="C4" s="2">
         <v>2547</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1">
-        <v>243.24700000000001</v>
+        <v>6</v>
+      </c>
+      <c r="B5" s="3">
+        <v>243247</v>
       </c>
       <c r="C5" s="2">
         <v>2191</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1">
-        <v>64.472999999999999</v>
+        <v>7</v>
+      </c>
+      <c r="B6" s="3">
+        <v>64473</v>
       </c>
       <c r="C6" s="2">
         <v>2149</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="B7" s="3">
+        <v>104099452</v>
       </c>
       <c r="C7" s="2">
         <v>1106</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="B8" s="3">
+        <v>91276115</v>
       </c>
       <c r="C8" s="2">
         <v>1028</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="B9" s="3">
+        <v>33406061</v>
       </c>
       <c r="C9" s="2">
         <v>860</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="B10" s="3">
+        <v>199812341</v>
       </c>
       <c r="C10" s="2">
         <v>829</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="1">
-        <v>343.709</v>
+        <v>12</v>
+      </c>
+      <c r="B11" s="3">
+        <v>343709</v>
       </c>
       <c r="C11" s="2">
         <v>700</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
+      </c>
+      <c r="B12" s="3">
+        <v>25351462</v>
       </c>
       <c r="C12" s="2">
         <v>573</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
+      </c>
+      <c r="B13" s="3">
+        <v>72147030</v>
       </c>
       <c r="C13" s="2">
         <v>555</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
+      </c>
+      <c r="B14" s="3">
+        <v>27743338</v>
       </c>
       <c r="C14" s="2">
         <v>551</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>16</v>
+      </c>
+      <c r="B15" s="3">
+        <v>32988134</v>
       </c>
       <c r="C15" s="2">
         <v>414</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
+      </c>
+      <c r="B16" s="3">
+        <v>31205576</v>
       </c>
       <c r="C16" s="2">
         <v>398</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>18</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1458545</v>
       </c>
       <c r="C17" s="2">
         <v>394</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
+      </c>
+      <c r="B18" s="3">
+        <v>112374333</v>
       </c>
       <c r="C18" s="2">
         <v>365</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>35</v>
+        <v>20</v>
+      </c>
+      <c r="B19" s="3">
+        <v>3673917</v>
       </c>
       <c r="C19" s="2">
         <v>350</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
+      </c>
+      <c r="B20" s="3">
+        <v>61095297</v>
       </c>
       <c r="C20" s="2">
         <v>319</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>39</v>
+        <v>22</v>
+      </c>
+      <c r="B21" s="3">
+        <v>84580777</v>
       </c>
       <c r="C21" s="2">
         <v>308</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>41</v>
+        <v>23</v>
+      </c>
+      <c r="B22" s="3">
+        <v>60439692</v>
       </c>
       <c r="C22" s="2">
         <v>308</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>43</v>
+        <v>24</v>
+      </c>
+      <c r="B23" s="3">
+        <v>35193978</v>
       </c>
       <c r="C23" s="2">
         <v>307</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>45</v>
+        <v>25</v>
+      </c>
+      <c r="B24" s="3">
+        <v>41974218</v>
       </c>
       <c r="C24" s="2">
         <v>270</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>47</v>
+        <v>26</v>
+      </c>
+      <c r="B25" s="3">
+        <v>72626809</v>
       </c>
       <c r="C25" s="2">
         <v>236</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
+      </c>
+      <c r="B26" s="3">
+        <v>68548437</v>
       </c>
       <c r="C26" s="2">
         <v>200</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>51</v>
+        <v>28</v>
+      </c>
+      <c r="B27" s="3">
+        <v>25545198</v>
       </c>
       <c r="C27" s="2">
         <v>189</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>53</v>
+        <v>29</v>
+      </c>
+      <c r="B28" s="3">
+        <v>10086292</v>
       </c>
       <c r="C28" s="2">
         <v>189</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>55</v>
+        <v>30</v>
+      </c>
+      <c r="B29" s="3">
+        <v>2966889</v>
       </c>
       <c r="C29" s="2">
         <v>132</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>57</v>
+        <v>31</v>
+      </c>
+      <c r="B30" s="3">
+        <v>2855794</v>
       </c>
       <c r="C30" s="2">
         <v>128</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>59</v>
+        <v>32</v>
+      </c>
+      <c r="B31" s="3">
+        <v>6864602</v>
       </c>
       <c r="C31" s="2">
         <v>123</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>61</v>
+        <v>33</v>
+      </c>
+      <c r="B32" s="3">
+        <v>1978502</v>
       </c>
       <c r="C32" s="2">
         <v>119</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B33" s="1">
-        <v>610.577</v>
+        <v>34</v>
+      </c>
+      <c r="B33" s="3">
+        <v>610577</v>
       </c>
       <c r="C33" s="2">
         <v>86</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>64</v>
+        <v>35</v>
+      </c>
+      <c r="B34" s="3">
+        <v>12541302</v>
       </c>
       <c r="C34" s="2">
         <v>56</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>66</v>
+        <v>36</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1097206</v>
       </c>
       <c r="C35" s="2">
         <v>52</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B36" s="1">
-        <v>380.58100000000002</v>
+        <v>37</v>
+      </c>
+      <c r="B36" s="3">
+        <v>380581</v>
       </c>
       <c r="C36" s="2">
         <v>46</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>69</v>
+        <v>38</v>
+      </c>
+      <c r="B37" s="3">
+        <v>1383727</v>
       </c>
       <c r="C37" s="2">
         <v>17</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="E37" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajustar las categorías de densidad poblacional
</commit_message>
<xml_diff>
--- a/data/india/population_density_IN.xlsx
+++ b/data/india/population_density_IN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776BF93C-7A6C-4977-8900-8A2714D30FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E9E5C4-413B-43FB-9C19-560100C772C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E7E294A-2B1B-457B-B9FE-B3636AF373CB}"/>
+    <workbookView xWindow="-390" yWindow="3195" windowWidth="21600" windowHeight="11385" xr2:uid="{7E7E294A-2B1B-457B-B9FE-B3636AF373CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
   <si>
     <t>State Name</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t>Very High</t>
+  </si>
+  <si>
+    <t>Very Low</t>
   </si>
 </sst>
 </file>
@@ -533,7 +539,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,7 +575,7 @@
         <v>11320</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E2" s="1"/>
     </row>
@@ -584,7 +590,7 @@
         <v>9258</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -944,7 +950,7 @@
         <v>189</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E27" s="1"/>
     </row>
@@ -959,7 +965,7 @@
         <v>189</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E28" s="1"/>
     </row>
@@ -974,7 +980,7 @@
         <v>132</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E29" s="1"/>
     </row>
@@ -989,7 +995,7 @@
         <v>128</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E30" s="1"/>
     </row>
@@ -1004,7 +1010,7 @@
         <v>123</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E31" s="1"/>
     </row>
@@ -1019,7 +1025,7 @@
         <v>119</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E32" s="1"/>
     </row>
@@ -1034,7 +1040,7 @@
         <v>86</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E33" s="1"/>
     </row>
@@ -1049,7 +1055,7 @@
         <v>56</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E34" s="1"/>
     </row>
@@ -1064,7 +1070,7 @@
         <v>52</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E35" s="1"/>
     </row>
@@ -1079,7 +1085,7 @@
         <v>46</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E36" s="1"/>
     </row>
@@ -1094,7 +1100,7 @@
         <v>17</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E37" s="1"/>
     </row>

</xml_diff>

<commit_message>
Modificar categorías de densidad poblacional
</commit_message>
<xml_diff>
--- a/data/india/population_density_IN.xlsx
+++ b/data/india/population_density_IN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0088F692-7175-40AF-A6F5-F1F7E30EEC05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00859115-EC75-4F55-88F0-65EBF71CC572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3195" windowWidth="21600" windowHeight="11385" xr2:uid="{7E7E294A-2B1B-457B-B9FE-B3636AF373CB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E7E294A-2B1B-457B-B9FE-B3636AF373CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="44">
   <si>
     <t>State Name</t>
   </si>
@@ -163,12 +163,6 @@
   </si>
   <si>
     <t>Low</t>
-  </si>
-  <si>
-    <t>Very High</t>
-  </si>
-  <si>
-    <t>Very Low</t>
   </si>
   <si>
     <t>Growth rate</t>
@@ -180,7 +174,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -243,7 +237,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda [0]" xfId="1" builtinId="7"/>
@@ -562,7 +556,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D37"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +577,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>39</v>
@@ -604,7 +598,7 @@
         <v>6.86</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -622,7 +616,7 @@
         <v>10.98</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -640,7 +634,7 @@
         <v>26.03</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -658,7 +652,7 @@
         <v>17.07</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -694,7 +688,7 @@
         <v>17.09</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F7" s="1"/>
     </row>
@@ -712,7 +706,7 @@
         <v>22.61</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F8" s="1"/>
     </row>
@@ -730,7 +724,7 @@
         <v>55.88</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F9" s="1"/>
     </row>
@@ -766,7 +760,7 @@
         <v>21.21</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F11" s="1"/>
     </row>
@@ -784,7 +778,7 @@
         <v>8.23</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -802,7 +796,7 @@
         <v>19.28</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F13" s="1"/>
     </row>
@@ -820,7 +814,7 @@
         <v>19.899999999999999</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14" s="1"/>
     </row>
@@ -838,7 +832,7 @@
         <v>12.94</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F15" s="1"/>
     </row>
@@ -856,7 +850,7 @@
         <v>23.64</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F16" s="1"/>
     </row>
@@ -874,7 +868,7 @@
         <v>22.42</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F17" s="1"/>
     </row>
@@ -892,7 +886,7 @@
         <v>15.6</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F18" s="1"/>
     </row>
@@ -910,7 +904,7 @@
         <v>4.91</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F19" s="1"/>
     </row>
@@ -946,7 +940,7 @@
         <v>20.350000000000001</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F21" s="1"/>
     </row>
@@ -964,7 +958,7 @@
         <v>15.99</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F22" s="1"/>
     </row>
@@ -982,7 +976,7 @@
         <v>24.5</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F23" s="1"/>
     </row>
@@ -1000,7 +994,7 @@
         <v>29.95</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F24" s="1"/>
     </row>
@@ -1018,7 +1012,7 @@
         <v>23.48</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F25" s="1"/>
     </row>
@@ -1036,7 +1030,7 @@
         <v>-0.57999999999999996</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F26" s="1"/>
     </row>
@@ -1054,7 +1048,7 @@
         <v>14.05</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F27" s="1"/>
     </row>
@@ -1090,7 +1084,7 @@
         <v>13.89</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F29" s="1"/>
     </row>
@@ -1108,7 +1102,7 @@
         <v>21.31</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F30" s="1"/>
     </row>
@@ -1126,7 +1120,7 @@
         <v>12.89</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F31" s="1"/>
     </row>
@@ -1144,7 +1138,7 @@
         <v>15.61</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F32" s="1"/>
     </row>
@@ -1162,7 +1156,7 @@
         <v>13.58</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F33" s="1"/>
     </row>
@@ -1180,7 +1174,7 @@
         <v>14.84</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F34" s="1"/>
     </row>
@@ -1198,7 +1192,7 @@
         <v>20.23</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F35" s="1"/>
     </row>
@@ -1216,7 +1210,7 @@
         <v>18.809999999999999</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F36" s="1"/>
     </row>

</xml_diff>

<commit_message>
Pequeño cambio en el estado Daman and Diu
</commit_message>
<xml_diff>
--- a/data/india/population_density_IN.xlsx
+++ b/data/india/population_density_IN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00859115-EC75-4F55-88F0-65EBF71CC572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E8FAC0-179B-4C48-A00C-78E2AA95808D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E7E294A-2B1B-457B-B9FE-B3636AF373CB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
   <si>
     <t>State Name</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Puducherry</t>
   </si>
   <si>
-    <t>Daman and Diu</t>
-  </si>
-  <si>
     <t>Lakshadweep</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>Uttar Pradesh</t>
   </si>
   <si>
-    <t>Dadra and Nagar Haveli</t>
-  </si>
-  <si>
     <t>Haryana</t>
   </si>
   <si>
@@ -166,6 +160,9 @@
   </si>
   <si>
     <t>Growth rate</t>
+  </si>
+  <si>
+    <t>Dadra and Nagar Haveli and Daman and Diu</t>
   </si>
 </sst>
 </file>
@@ -556,13 +553,14 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="46.140625" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -577,16 +575,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="3">
         <v>380581</v>
@@ -598,13 +596,13 @@
         <v>6.86</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" s="3">
         <v>84580777</v>
@@ -616,13 +614,13 @@
         <v>10.98</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" s="3">
         <v>1383727</v>
@@ -634,13 +632,13 @@
         <v>26.03</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3">
         <v>31205576</v>
@@ -652,13 +650,13 @@
         <v>17.07</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="3">
         <v>104099452</v>
@@ -670,7 +668,7 @@
         <v>25.4</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -688,13 +686,13 @@
         <v>17.09</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="3">
         <v>25545198</v>
@@ -706,112 +704,113 @@
         <v>22.61</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="B9" s="3">
-        <v>343709</v>
+        <f>343709+243247</f>
+        <v>586956</v>
       </c>
       <c r="C9" s="2">
-        <v>700</v>
+        <f>700+2191</f>
+        <v>2891</v>
       </c>
       <c r="D9" s="4">
         <v>55.88</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B10" s="3">
-        <v>243247</v>
+        <v>16787941</v>
       </c>
       <c r="C10" s="2">
-        <v>2191</v>
+        <v>11320</v>
       </c>
       <c r="D10" s="4">
-        <v>53.76</v>
+        <v>21.21</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="1"/>
+        <v>38</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B11" s="3">
-        <v>16787941</v>
+        <v>1458545</v>
       </c>
       <c r="C11" s="2">
-        <v>11320</v>
+        <v>394</v>
       </c>
       <c r="D11" s="4">
-        <v>21.21</v>
+        <v>8.23</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B12" s="3">
-        <v>1458545</v>
+        <v>60439692</v>
       </c>
       <c r="C12" s="2">
-        <v>394</v>
+        <v>308</v>
       </c>
       <c r="D12" s="4">
-        <v>8.23</v>
+        <v>19.28</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B13" s="3">
-        <v>60439692</v>
+        <v>25351462</v>
       </c>
       <c r="C13" s="2">
-        <v>308</v>
+        <v>573</v>
       </c>
       <c r="D13" s="4">
-        <v>19.28</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B14" s="3">
-        <v>25351462</v>
+        <v>6864602</v>
       </c>
       <c r="C14" s="2">
-        <v>573</v>
+        <v>123</v>
       </c>
       <c r="D14" s="4">
-        <v>19.899999999999999</v>
+        <v>12.94</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>40</v>
@@ -820,376 +819,376 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B15" s="3">
-        <v>6864602</v>
+        <v>12541302</v>
       </c>
       <c r="C15" s="2">
-        <v>123</v>
+        <v>56</v>
       </c>
       <c r="D15" s="4">
-        <v>12.94</v>
+        <v>23.64</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B16" s="3">
-        <v>12541302</v>
+        <v>32988134</v>
       </c>
       <c r="C16" s="2">
-        <v>56</v>
+        <v>414</v>
       </c>
       <c r="D16" s="4">
-        <v>23.64</v>
+        <v>22.42</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B17" s="3">
-        <v>32988134</v>
+        <v>61095297</v>
       </c>
       <c r="C17" s="2">
-        <v>414</v>
+        <v>319</v>
       </c>
       <c r="D17" s="4">
-        <v>22.42</v>
+        <v>15.6</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B18" s="3">
-        <v>61095297</v>
+        <v>33406061</v>
       </c>
       <c r="C18" s="2">
-        <v>319</v>
+        <v>860</v>
       </c>
       <c r="D18" s="4">
-        <v>15.6</v>
+        <v>4.91</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B19" s="3">
-        <v>33406061</v>
+        <v>64473</v>
       </c>
       <c r="C19" s="2">
-        <v>860</v>
+        <v>2149</v>
       </c>
       <c r="D19" s="4">
-        <v>4.91</v>
+        <v>6.3</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B20" s="3">
-        <v>64473</v>
+        <v>72626809</v>
       </c>
       <c r="C20" s="2">
-        <v>2149</v>
+        <v>236</v>
       </c>
       <c r="D20" s="4">
-        <v>6.3</v>
+        <v>20.350000000000001</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B21" s="3">
-        <v>72626809</v>
+        <v>112374333</v>
       </c>
       <c r="C21" s="2">
-        <v>236</v>
+        <v>365</v>
       </c>
       <c r="D21" s="4">
-        <v>20.350000000000001</v>
+        <v>15.99</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B22" s="3">
-        <v>112374333</v>
+        <v>2855794</v>
       </c>
       <c r="C22" s="2">
-        <v>365</v>
+        <v>128</v>
       </c>
       <c r="D22" s="4">
-        <v>15.99</v>
+        <v>24.5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B23" s="3">
-        <v>2855794</v>
+        <v>2966889</v>
       </c>
       <c r="C23" s="2">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D23" s="4">
-        <v>24.5</v>
+        <v>29.95</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B24" s="3">
-        <v>2966889</v>
+        <v>1097206</v>
       </c>
       <c r="C24" s="2">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="D24" s="4">
-        <v>29.95</v>
+        <v>23.48</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B25" s="3">
-        <v>1097206</v>
+        <v>1978502</v>
       </c>
       <c r="C25" s="2">
-        <v>52</v>
+        <v>119</v>
       </c>
       <c r="D25" s="4">
-        <v>23.48</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B26" s="3">
-        <v>1978502</v>
+        <v>41974218</v>
       </c>
       <c r="C26" s="2">
-        <v>119</v>
+        <v>270</v>
       </c>
       <c r="D26" s="4">
-        <v>-0.57999999999999996</v>
+        <v>14.05</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="B27" s="3">
-        <v>41974218</v>
+        <v>1247953</v>
       </c>
       <c r="C27" s="2">
-        <v>270</v>
+        <v>2547</v>
       </c>
       <c r="D27" s="4">
-        <v>14.05</v>
+        <v>28.08</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B28" s="3">
-        <v>1247953</v>
+        <v>27743338</v>
       </c>
       <c r="C28" s="2">
-        <v>2547</v>
+        <v>551</v>
       </c>
       <c r="D28" s="4">
-        <v>28.08</v>
+        <v>13.89</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B29" s="3">
-        <v>27743338</v>
+        <v>68548437</v>
       </c>
       <c r="C29" s="2">
-        <v>551</v>
+        <v>200</v>
       </c>
       <c r="D29" s="4">
-        <v>13.89</v>
+        <v>21.31</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B30" s="3">
-        <v>68548437</v>
+        <v>610577</v>
       </c>
       <c r="C30" s="2">
-        <v>200</v>
+        <v>86</v>
       </c>
       <c r="D30" s="4">
-        <v>21.31</v>
+        <v>12.89</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="B31" s="3">
-        <v>610577</v>
+        <v>72147030</v>
       </c>
       <c r="C31" s="2">
-        <v>86</v>
+        <v>555</v>
       </c>
       <c r="D31" s="4">
-        <v>12.89</v>
+        <v>15.61</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B32" s="3">
-        <v>72147030</v>
+        <v>35193978</v>
       </c>
       <c r="C32" s="2">
-        <v>555</v>
+        <v>307</v>
       </c>
       <c r="D32" s="4">
-        <v>15.61</v>
+        <v>13.58</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B33" s="3">
-        <v>35193978</v>
+        <v>3673917</v>
       </c>
       <c r="C33" s="2">
-        <v>307</v>
+        <v>350</v>
       </c>
       <c r="D33" s="4">
-        <v>13.58</v>
+        <v>14.84</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B34" s="3">
-        <v>3673917</v>
+        <v>199812341</v>
       </c>
       <c r="C34" s="2">
-        <v>350</v>
+        <v>829</v>
       </c>
       <c r="D34" s="4">
-        <v>14.84</v>
+        <v>20.23</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B35" s="3">
-        <v>199812341</v>
+        <v>10086292</v>
       </c>
       <c r="C35" s="2">
-        <v>829</v>
+        <v>189</v>
       </c>
       <c r="D35" s="4">
-        <v>20.23</v>
+        <v>18.809999999999999</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>40</v>
@@ -1198,43 +1197,28 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B36" s="3">
-        <v>10086292</v>
+        <v>91276115</v>
       </c>
       <c r="C36" s="2">
-        <v>189</v>
+        <v>1028</v>
       </c>
       <c r="D36" s="4">
-        <v>18.809999999999999</v>
+        <v>13.84</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" s="3">
-        <v>91276115</v>
-      </c>
-      <c r="C37" s="2">
-        <v>1028</v>
-      </c>
-      <c r="D37" s="4">
-        <v>13.84</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="F37" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E37">
-    <sortCondition ref="A1:A37"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E36">
+    <sortCondition ref="A1:A36"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>